<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@2ecc0569988186c3a9635dfcc337f620cfb4510e 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-average-blood-pressure.xlsx
+++ b/StructureDefinition-us-core-average-blood-pressure.xlsx
@@ -901,8 +901,8 @@
 </t>
   </si>
   <si>
-    <t>dateTime
-Period</t>
+    <t xml:space="preserve">Period
+</t>
   </si>
   <si>
     <t>(USCDI) clinically relevant time-period for the average of blood pressure (BP) readings</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@3523601ddafde83145c9cd712fff7acb0de07ded 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-average-blood-pressure.xlsx
+++ b/StructureDefinition-us-core-average-blood-pressure.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3646" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3646" uniqueCount="579">
   <si>
     <t>Property</t>
   </si>
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-02</t>
+    <t>2023-10-11</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -772,7 +772,7 @@
 </t>
   </si>
   <si>
-    <t>(USCDI) Average Blood Pressure</t>
+    <t>Average Blood Pressure</t>
   </si>
   <si>
     <t>Coded Responses from C-CDA Vital Sign Results.</t>
@@ -915,7 +915,7 @@
 </t>
   </si>
   <si>
-    <t>(USCDI) clinically relevant time-period for the average of blood pressure (BP) readings</t>
+    <t>clinically relevant time-period for the average of blood pressure (BP) readings</t>
   </si>
   <si>
     <t>Often just a dateTime for Vital Signs.</t>
@@ -1468,7 +1468,7 @@
     <t>2</t>
   </si>
   <si>
-    <t>(USCDI) Component observations</t>
+    <t>Component observations</t>
   </si>
   <si>
     <t>Used when reporting component observation such as systolic and diastolic blood pressure.</t>
@@ -1576,7 +1576,7 @@
     <t>systolic</t>
   </si>
   <si>
-    <t>(USCDI) Average Systolic Blood Pressure</t>
+    <t>Average Systolic Blood Pressure</t>
   </si>
   <si>
     <t>Observation.component:systolic.id</t>
@@ -1591,7 +1591,7 @@
     <t>Observation.component:systolic.code</t>
   </si>
   <si>
-    <t>(USCDI) Average Systolic Blood Pressure Code</t>
+    <t>Average Systolic Blood Pressure Code</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
@@ -1609,6 +1609,9 @@
 </t>
   </si>
   <si>
+    <t>Vital Sign Component Value</t>
+  </si>
+  <si>
     <t>Observation.component:systolic.value[x].id</t>
   </si>
   <si>
@@ -1631,7 +1634,7 @@
 </t>
   </si>
   <si>
-    <t>(USCDI) Numerical value (with implicit precision)</t>
+    <t>Numerical value (with implicit precision)</t>
   </si>
   <si>
     <t>The value of the measured amount. The value includes an implicit precision in the presentation of the value.</t>
@@ -1691,7 +1694,7 @@
     <t>Observation.component.value[x].unit</t>
   </si>
   <si>
-    <t>(USCDI) Unit representation</t>
+    <t>Unit representation</t>
   </si>
   <si>
     <t>A human-readable form of the unit.</t>
@@ -1715,7 +1718,7 @@
     <t>Observation.component.value[x].system</t>
   </si>
   <si>
-    <t>(USCDI) System that defines coded unit form</t>
+    <t>System that defines coded unit form</t>
   </si>
   <si>
     <t>The identification of the system that provides the coded form of the unit.</t>
@@ -1743,7 +1746,7 @@
     <t>Observation.component.value[x].code</t>
   </si>
   <si>
-    <t>(USCDI) Coded form of the unit</t>
+    <t>Coded form of the unit</t>
   </si>
   <si>
     <t>A computer processable form of the unit in some unit representation system.</t>
@@ -1779,7 +1782,7 @@
     <t>diastolic</t>
   </si>
   <si>
-    <t>(USCDI) Average Diastolic Blood Pressure</t>
+    <t>Average Diastolic Blood Pressure</t>
   </si>
   <si>
     <t>Observation.component:diastolic.id</t>
@@ -1794,7 +1797,7 @@
     <t>Observation.component:diastolic.code</t>
   </si>
   <si>
-    <t>(USCDI) Average Diastolic Blood Pressure Code</t>
+    <t>Average Diastolic Blood Pressure Code</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
@@ -10321,7 +10324,7 @@
         <v>503</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>479</v>
+        <v>504</v>
       </c>
       <c r="M68" t="s" s="2">
         <v>480</v>
@@ -10414,10 +10417,10 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -10532,10 +10535,10 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10652,10 +10655,10 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10678,19 +10681,19 @@
         <v>50</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="N71" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="O71" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="P71" t="s" s="2">
         <v>40</v>
@@ -10739,7 +10742,7 @@
         <v>40</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>38</v>
@@ -10760,10 +10763,10 @@
         <v>40</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="AN71" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="AO71" t="s" s="2">
         <v>40</v>
@@ -10774,10 +10777,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10803,20 +10806,20 @@
         <v>69</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="P72" t="s" s="2">
         <v>40</v>
       </c>
       <c r="Q72" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="R72" t="s" s="2">
         <v>40</v>
@@ -10840,10 +10843,10 @@
         <v>138</v>
       </c>
       <c r="Y72" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="Z72" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="AA72" t="s" s="2">
         <v>40</v>
@@ -10861,7 +10864,7 @@
         <v>40</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>38</v>
@@ -10882,10 +10885,10 @@
         <v>40</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="AN72" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="AO72" t="s" s="2">
         <v>40</v>
@@ -10896,10 +10899,10 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10925,14 +10928,14 @@
         <v>161</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="N73" s="2"/>
       <c r="O73" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="P73" t="s" s="2">
         <v>40</v>
@@ -10981,7 +10984,7 @@
         <v>40</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>38</v>
@@ -11002,10 +11005,10 @@
         <v>40</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="AN73" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="AO73" t="s" s="2">
         <v>40</v>
@@ -11016,10 +11019,10 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -11045,21 +11048,21 @@
         <v>63</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="P74" t="s" s="2">
         <v>40</v>
       </c>
       <c r="Q74" s="2"/>
       <c r="R74" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="S74" t="s" s="2">
         <v>40</v>
@@ -11101,7 +11104,7 @@
         <v>40</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>38</v>
@@ -11110,7 +11113,7 @@
         <v>49</v>
       </c>
       <c r="AI74" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="AJ74" t="s" s="2">
         <v>61</v>
@@ -11122,10 +11125,10 @@
         <v>40</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="AN74" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="AO74" t="s" s="2">
         <v>40</v>
@@ -11136,10 +11139,10 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -11165,23 +11168,23 @@
         <v>69</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="N75" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="O75" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="P75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="Q75" s="2"/>
       <c r="R75" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="S75" t="s" s="2">
         <v>40</v>
@@ -11223,7 +11226,7 @@
         <v>40</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>38</v>
@@ -11244,10 +11247,10 @@
         <v>40</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="AN75" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="AO75" t="s" s="2">
         <v>40</v>
@@ -11258,7 +11261,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B76" t="s" s="2">
         <v>484</v>
@@ -11380,7 +11383,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B77" t="s" s="2">
         <v>489</v>
@@ -11502,7 +11505,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B78" t="s" s="2">
         <v>490</v>
@@ -11624,13 +11627,13 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B79" t="s" s="2">
         <v>459</v>
       </c>
       <c r="C79" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D79" t="s" s="2">
         <v>40</v>
@@ -11655,7 +11658,7 @@
         <v>394</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="M79" t="s" s="2">
         <v>462</v>
@@ -11748,7 +11751,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B80" t="s" s="2">
         <v>469</v>
@@ -11866,7 +11869,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B81" t="s" s="2">
         <v>470</v>
@@ -11986,7 +11989,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B82" t="s" s="2">
         <v>471</v>
@@ -12108,7 +12111,7 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B83" t="s" s="2">
         <v>472</v>
@@ -12137,7 +12140,7 @@
         <v>146</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="M83" t="s" s="2">
         <v>474</v>
@@ -12156,7 +12159,7 @@
         <v>40</v>
       </c>
       <c r="S83" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="T83" t="s" s="2">
         <v>40</v>
@@ -12230,7 +12233,7 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B84" t="s" s="2">
         <v>478</v>
@@ -12259,7 +12262,7 @@
         <v>503</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>479</v>
+        <v>504</v>
       </c>
       <c r="M84" t="s" s="2">
         <v>480</v>
@@ -12352,10 +12355,10 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -12470,10 +12473,10 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12590,10 +12593,10 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
@@ -12616,19 +12619,19 @@
         <v>50</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="N87" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="O87" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="P87" t="s" s="2">
         <v>40</v>
@@ -12677,7 +12680,7 @@
         <v>40</v>
       </c>
       <c r="AF87" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="AG87" t="s" s="2">
         <v>38</v>
@@ -12698,10 +12701,10 @@
         <v>40</v>
       </c>
       <c r="AM87" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="AN87" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="AO87" t="s" s="2">
         <v>40</v>
@@ -12712,10 +12715,10 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
@@ -12741,20 +12744,20 @@
         <v>69</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="M88" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="N88" s="2"/>
       <c r="O88" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="P88" t="s" s="2">
         <v>40</v>
       </c>
       <c r="Q88" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="R88" t="s" s="2">
         <v>40</v>
@@ -12778,10 +12781,10 @@
         <v>138</v>
       </c>
       <c r="Y88" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="Z88" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="AA88" t="s" s="2">
         <v>40</v>
@@ -12799,7 +12802,7 @@
         <v>40</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>38</v>
@@ -12820,10 +12823,10 @@
         <v>40</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="AN88" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="AO88" t="s" s="2">
         <v>40</v>
@@ -12834,10 +12837,10 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
@@ -12863,14 +12866,14 @@
         <v>161</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="N89" s="2"/>
       <c r="O89" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="P89" t="s" s="2">
         <v>40</v>
@@ -12919,7 +12922,7 @@
         <v>40</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="AG89" t="s" s="2">
         <v>38</v>
@@ -12940,10 +12943,10 @@
         <v>40</v>
       </c>
       <c r="AM89" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="AN89" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="AO89" t="s" s="2">
         <v>40</v>
@@ -12954,10 +12957,10 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
@@ -12983,21 +12986,21 @@
         <v>63</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="N90" s="2"/>
       <c r="O90" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="P90" t="s" s="2">
         <v>40</v>
       </c>
       <c r="Q90" s="2"/>
       <c r="R90" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="S90" t="s" s="2">
         <v>40</v>
@@ -13039,7 +13042,7 @@
         <v>40</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>38</v>
@@ -13048,7 +13051,7 @@
         <v>49</v>
       </c>
       <c r="AI90" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="AJ90" t="s" s="2">
         <v>61</v>
@@ -13060,10 +13063,10 @@
         <v>40</v>
       </c>
       <c r="AM90" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="AN90" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="AO90" t="s" s="2">
         <v>40</v>
@@ -13074,10 +13077,10 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
@@ -13103,23 +13106,23 @@
         <v>69</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="N91" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="O91" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="P91" t="s" s="2">
         <v>40</v>
       </c>
       <c r="Q91" s="2"/>
       <c r="R91" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="S91" t="s" s="2">
         <v>40</v>
@@ -13161,7 +13164,7 @@
         <v>40</v>
       </c>
       <c r="AF91" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="AG91" t="s" s="2">
         <v>38</v>
@@ -13182,10 +13185,10 @@
         <v>40</v>
       </c>
       <c r="AM91" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="AN91" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="AO91" t="s" s="2">
         <v>40</v>
@@ -13196,7 +13199,7 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B92" t="s" s="2">
         <v>484</v>
@@ -13318,7 +13321,7 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B93" t="s" s="2">
         <v>489</v>
@@ -13440,7 +13443,7 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B94" t="s" s="2">
         <v>490</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@532a38ddcd1ea7ef74c69262f63b7afc59b37e88 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-average-blood-pressure.xlsx
+++ b/StructureDefinition-us-core-average-blood-pressure.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-12</t>
+    <t>2023-10-19</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -911,8 +911,8 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Period
-</t>
+    <t>dateTime
+Period</t>
   </si>
   <si>
     <t>clinically relevant time-period for the average of blood pressure (BP) readings</t>

</xml_diff>